<commit_message>
- first working on Pi - introducing Pin enum
git-svn-id: file:///C/Home/chuma/Data/BackUp/.svnRepo/trunk/HomeAutomation@80 155b416f-c310-5041-93e3-512504897193
</commit_message>
<xml_diff>
--- a/packetCounting.xlsx
+++ b/packetCounting.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="21915" windowHeight="8070" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="21915" windowHeight="8070"/>
   </bookViews>
   <sheets>
-    <sheet name="crc2" sheetId="2" r:id="rId1"/>
+    <sheet name="Packet CRC" sheetId="2" r:id="rId1"/>
     <sheet name="CAN Clock" sheetId="3" r:id="rId2"/>
     <sheet name="PWM" sheetId="4" r:id="rId3"/>
     <sheet name="Display" sheetId="5" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>CRC</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>F0</t>
   </si>
 </sst>
 </file>
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -297,6 +303,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -304,7 +313,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G32"/>
+  <dimension ref="A3:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,12 +695,12 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -710,8 +719,12 @@
       <c r="G4">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>MOD(J16+128,128)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -730,8 +743,12 @@
       <c r="G5">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f>MOD(J17+128,128)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -750,8 +767,12 @@
       <c r="G6">
         <v>203</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f>MOD(J18+128,128)+128</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -770,8 +791,11 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -790,8 +814,11 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -810,8 +837,11 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -830,8 +860,11 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
@@ -851,17 +884,20 @@
       <c r="G11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
@@ -885,8 +921,12 @@
         <f>G11+2</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f>H11+2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>0</v>
       </c>
@@ -907,11 +947,22 @@
         <v>153</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16" si="1">MOD(G4, 128)+128</f>
+        <f t="shared" ref="G16:H16" si="1">MOD(G4, 128)+128</f>
         <v>153</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16">
+        <f>HEX2DEC(I16)</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>1</v>
       </c>
@@ -932,11 +983,22 @@
         <v>162</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17" si="2">MOD(G5, 128)+128</f>
+        <f t="shared" ref="G17:H17" si="2">MOD(G5, 128)+128</f>
         <v>162</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J20" si="3">HEX2DEC(I17)</f>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2</v>
       </c>
@@ -957,11 +1019,22 @@
         <v>128</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18" si="3">MOD(G6, 128)+128</f>
+        <f t="shared" ref="G18:H18" si="4">MOD(G6, 128)+128</f>
         <v>203</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>3</v>
       </c>
@@ -982,11 +1055,22 @@
         <v>128</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" ref="G19" si="4">MOD(G7, 128)+128</f>
+        <f t="shared" ref="G19:H19" si="5">MOD(G7, 128)+128</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="4">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="I19" s="19">
+        <v>84</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>4</v>
       </c>
@@ -1007,11 +1091,22 @@
         <v>128</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" ref="G20" si="5">MOD(G8, 128)+128</f>
+        <f t="shared" ref="G20:H20" si="6">MOD(G8, 128)+128</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="4">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="I20" s="19">
+        <v>25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>5</v>
       </c>
@@ -1032,11 +1127,15 @@
         <v>128</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" ref="G21" si="6">MOD(G9, 128)+128</f>
+        <f t="shared" ref="G21:H21" si="7">MOD(G9, 128)+128</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="4">
+        <f t="shared" si="7"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>6</v>
       </c>
@@ -1057,11 +1156,15 @@
         <v>128</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" ref="G22" si="7">MOD(G10, 128)+128</f>
+        <f t="shared" ref="G22:H22" si="8">MOD(G10, 128)+128</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="4">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>1</v>
       </c>
@@ -1085,8 +1188,12 @@
         <f>SUM(ROUNDDOWN(G4/128,0)*1,ROUNDDOWN(G5/128,0)*2,ROUNDDOWN(G6/128,0)*4,ROUNDDOWN(G7/128,0)*8,ROUNDDOWN(G8/128,0)*16,ROUNDDOWN(G9/128,0)*32,ROUNDDOWN(G10/128,0)*64,128)</f>
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f>SUM(ROUNDDOWN(H4/128,0)*1,ROUNDDOWN(H5/128,0)*2,ROUNDDOWN(H6/128,0)*4,ROUNDDOWN(H7/128,0)*8,ROUNDDOWN(H8/128,0)*16,ROUNDDOWN(H9/128,0)*32,ROUNDDOWN(H10/128,0)*64,128)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
@@ -1110,8 +1217,12 @@
         <f>MOD(SUM(G16:G23,G11),128)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f>MOD(SUM(H16:H23,H11),128)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1130,8 +1241,11 @@
       <c r="G26">
         <v>335</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1147,8 +1261,11 @@
       <c r="G27">
         <v>314</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1164,12 +1281,15 @@
       <c r="G28">
         <v>371</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="H28">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="17"/>
       <c r="C29">
         <v>700</v>
       </c>
@@ -1182,8 +1302,11 @@
       <c r="G29">
         <v>523</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>696</v>
       </c>
@@ -1196,8 +1319,11 @@
       <c r="G30">
         <v>515</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>552</v>
       </c>
@@ -1210,8 +1336,11 @@
       <c r="G31">
         <v>400</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E32">
         <f>1000/30</f>
         <v>33.333333333333336</v>
@@ -1361,14 +1490,14 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="17"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
@@ -1515,21 +1644,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1549,13 +1678,13 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>4</v>
       </c>
     </row>
@@ -1563,13 +1692,13 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>7</v>
       </c>
     </row>
@@ -1577,13 +1706,13 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>6</v>
       </c>
     </row>
@@ -1591,13 +1720,13 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>5</v>
       </c>
     </row>
@@ -1605,13 +1734,13 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>3</v>
       </c>
     </row>
@@ -1619,13 +1748,13 @@
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>2</v>
       </c>
       <c r="F10" s="1">
@@ -1663,13 +1792,13 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>1</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -1710,13 +1839,13 @@
       <c r="A12">
         <v>21</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -1757,13 +1886,13 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>11</v>
       </c>
       <c r="E13" s="15" t="s">
@@ -1804,13 +1933,13 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>12</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -1851,13 +1980,13 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>13</v>
       </c>
       <c r="E15" s="15" t="s">
@@ -1898,13 +2027,13 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="16">
         <v>14</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -1945,13 +2074,13 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>10</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -1992,13 +2121,13 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <v>9</v>
       </c>
       <c r="E18" s="15" t="s">

</xml_diff>